<commit_message>
Added (static) 3D maze rendering.
</commit_message>
<xml_diff>
--- a/View Worksheet.xlsx
+++ b/View Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\getzi\Documents\Programming\StoneQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF50ED57-4713-4DE2-B4A2-0340E708AC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191EB9D9-7C14-48AB-BB8F-1D6B2A9483D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27090" yWindow="60" windowWidth="21600" windowHeight="11385" xr2:uid="{F8B1DF8C-620C-4209-94E3-2220A84177B2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="11">
   <si>
     <t>/</t>
   </si>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E896FD88-8069-4F5F-B4CA-DD975BD79C44}">
   <dimension ref="A1:AF119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,9 +660,11 @@
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="K3" s="14" t="s">
+        <v>2</v>
+      </c>
       <c r="L3" s="15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>3</v>
@@ -729,10 +731,10 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="J4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13"/>
       <c r="L4" s="16"/>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -766,10 +768,10 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="I5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="16"/>
       <c r="M5" s="16"/>
@@ -805,10 +807,10 @@
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="15" t="s">
-        <v>0</v>
-      </c>
+      <c r="H6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="17"/>
@@ -844,10 +846,10 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="G7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
@@ -881,10 +883,10 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="F8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
@@ -920,10 +922,10 @@
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="15" t="s">
-        <v>0</v>
-      </c>
+      <c r="E9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="17"/>
@@ -959,10 +961,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="D10" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="13"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -996,10 +998,10 @@
       <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="C11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>

</xml_diff>

<commit_message>
Dynamic (but very buggy) 3D rendering.
</commit_message>
<xml_diff>
--- a/View Worksheet.xlsx
+++ b/View Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\getzi\Documents\Programming\StoneQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191EB9D9-7C14-48AB-BB8F-1D6B2A9483D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073B9E02-4156-41B3-9AC3-830C3B8A5CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27090" yWindow="60" windowWidth="21600" windowHeight="11385" xr2:uid="{F8B1DF8C-620C-4209-94E3-2220A84177B2}"/>
+    <workbookView xWindow="-24210" yWindow="1830" windowWidth="21600" windowHeight="11385" xr2:uid="{F8B1DF8C-620C-4209-94E3-2220A84177B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="11">
   <si>
     <t>/</t>
   </si>
@@ -211,14 +211,14 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E896FD88-8069-4F5F-B4CA-DD975BD79C44}">
-  <dimension ref="A1:AF119"/>
+  <dimension ref="A1:AF134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="AH139" sqref="AH139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,8 +547,9 @@
     <col min="6" max="8" width="1.7109375" style="1" customWidth="1"/>
     <col min="9" max="11" width="1.7109375" style="8" customWidth="1"/>
     <col min="12" max="14" width="1.7109375" style="1" customWidth="1"/>
-    <col min="15" max="17" width="1.7109375" style="8" customWidth="1"/>
-    <col min="18" max="20" width="1.7109375" style="1" customWidth="1"/>
+    <col min="15" max="17" width="1.7109375" style="8" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="1.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="1.7109375" style="1" customWidth="1"/>
     <col min="21" max="23" width="1.7109375" style="8" customWidth="1"/>
     <col min="24" max="26" width="1.7109375" style="1" customWidth="1"/>
     <col min="27" max="29" width="1.7109375" style="8" customWidth="1"/>
@@ -558,7 +559,7 @@
       <c r="L1" s="1">
         <v>1</v>
       </c>
-      <c r="V1" s="8">
+      <c r="Z1" s="8">
         <v>2</v>
       </c>
     </row>
@@ -612,41 +613,41 @@
         <v>6</v>
       </c>
       <c r="S2" s="1">
+        <v>3</v>
+      </c>
+      <c r="T2" s="1">
+        <v>4</v>
+      </c>
+      <c r="U2" s="8">
+        <v>5</v>
+      </c>
+      <c r="V2" s="8">
+        <v>6</v>
+      </c>
+      <c r="W2" s="8">
         <v>7</v>
       </c>
-      <c r="T2" s="1">
+      <c r="X2" s="1">
         <v>8</v>
       </c>
-      <c r="U2" s="8">
+      <c r="Y2" s="1">
         <v>9</v>
       </c>
-      <c r="V2" s="8">
-        <v>0</v>
-      </c>
-      <c r="W2" s="8">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>3</v>
-      </c>
       <c r="Z2" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB2" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC2" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6">
@@ -693,34 +694,20 @@
       <c r="U3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="X3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="19" t="s">
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="6">
         <v>2</v>
       </c>
@@ -755,10 +742,10 @@
       <c r="AA4" s="11"/>
       <c r="AB4" s="11"/>
       <c r="AC4" s="11"/>
-      <c r="AD4" s="19"/>
+      <c r="AD4" s="21"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="6">
         <v>3</v>
       </c>
@@ -793,10 +780,10 @@
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
-      <c r="AD5" s="19"/>
+      <c r="AD5" s="21"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="5">
@@ -833,12 +820,12 @@
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
-      <c r="AD6" s="19" t="s">
+      <c r="AD6" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -873,10 +860,10 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
       <c r="AC7" s="12"/>
-      <c r="AD7" s="19"/>
+      <c r="AD7" s="21"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -911,10 +898,10 @@
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
       <c r="AC8" s="12"/>
-      <c r="AD8" s="19"/>
+      <c r="AD8" s="21"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2">
@@ -951,12 +938,12 @@
       </c>
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
-      <c r="AD9" s="19" t="s">
+      <c r="AD9" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -991,10 +978,10 @@
         <v>1</v>
       </c>
       <c r="AC10" s="14"/>
-      <c r="AD10" s="19"/>
+      <c r="AD10" s="21"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -1029,13 +1016,13 @@
       <c r="AC11" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="AD11" s="19"/>
+      <c r="AD11" s="21"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="L17" s="1">
         <v>1</v>
       </c>
-      <c r="V17" s="8">
+      <c r="Z17" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1089,41 +1076,41 @@
         <v>6</v>
       </c>
       <c r="S18" s="1">
+        <v>3</v>
+      </c>
+      <c r="T18" s="1">
+        <v>4</v>
+      </c>
+      <c r="U18" s="8">
+        <v>5</v>
+      </c>
+      <c r="V18" s="8">
+        <v>6</v>
+      </c>
+      <c r="W18" s="8">
         <v>7</v>
       </c>
-      <c r="T18" s="1">
+      <c r="X18" s="1">
         <v>8</v>
       </c>
-      <c r="U18" s="8">
+      <c r="Y18" s="1">
         <v>9</v>
       </c>
-      <c r="V18" s="8">
-        <v>0</v>
-      </c>
-      <c r="W18" s="8">
-        <v>1</v>
-      </c>
-      <c r="X18" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y18" s="1">
-        <v>3</v>
-      </c>
       <c r="Z18" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB18" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC18" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="6">
@@ -1178,12 +1165,12 @@
       <c r="AA19" s="11"/>
       <c r="AB19" s="11"/>
       <c r="AC19" s="11"/>
-      <c r="AD19" s="19" t="s">
+      <c r="AD19" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="6">
         <v>2</v>
       </c>
@@ -1218,10 +1205,10 @@
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
       <c r="AC20" s="11"/>
-      <c r="AD20" s="19"/>
+      <c r="AD20" s="21"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="6">
         <v>3</v>
       </c>
@@ -1256,10 +1243,10 @@
       <c r="AA21" s="11"/>
       <c r="AB21" s="11"/>
       <c r="AC21" s="11"/>
-      <c r="AD21" s="19"/>
+      <c r="AD21" s="21"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="5">
@@ -1296,12 +1283,12 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
-      <c r="AD22" s="19" t="s">
+      <c r="AD22" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="5">
         <v>5</v>
       </c>
@@ -1336,10 +1323,10 @@
       <c r="AA23" s="12"/>
       <c r="AB23" s="12"/>
       <c r="AC23" s="12"/>
-      <c r="AD23" s="19"/>
+      <c r="AD23" s="21"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5">
         <v>6</v>
       </c>
@@ -1374,10 +1361,10 @@
       <c r="AA24" s="12"/>
       <c r="AB24" s="12"/>
       <c r="AC24" s="12"/>
-      <c r="AD24" s="19"/>
+      <c r="AD24" s="21"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="2">
@@ -1414,12 +1401,12 @@
       </c>
       <c r="AB25" s="13"/>
       <c r="AC25" s="13"/>
-      <c r="AD25" s="19" t="s">
+      <c r="AD25" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="2">
         <v>8</v>
       </c>
@@ -1454,10 +1441,10 @@
         <v>1</v>
       </c>
       <c r="AC26" s="14"/>
-      <c r="AD26" s="19"/>
+      <c r="AD26" s="21"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="2">
         <v>9</v>
       </c>
@@ -1492,13 +1479,13 @@
       <c r="AC27" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="AD27" s="19"/>
+      <c r="AD27" s="21"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="L30" s="1">
         <v>1</v>
       </c>
-      <c r="V30" s="8">
+      <c r="Z30" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1512,7 +1499,7 @@
       <c r="E31" s="8">
         <v>3</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="1">
         <v>4</v>
       </c>
       <c r="G31" s="1">
@@ -1552,41 +1539,41 @@
         <v>6</v>
       </c>
       <c r="S31" s="1">
+        <v>3</v>
+      </c>
+      <c r="T31" s="1">
+        <v>4</v>
+      </c>
+      <c r="U31" s="8">
+        <v>5</v>
+      </c>
+      <c r="V31" s="8">
+        <v>6</v>
+      </c>
+      <c r="W31" s="8">
         <v>7</v>
       </c>
-      <c r="T31" s="1">
+      <c r="X31" s="1">
         <v>8</v>
       </c>
-      <c r="U31" s="8">
+      <c r="Y31" s="1">
         <v>9</v>
       </c>
-      <c r="V31" s="8">
-        <v>0</v>
-      </c>
-      <c r="W31" s="8">
-        <v>1</v>
-      </c>
-      <c r="X31" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y31" s="1">
-        <v>3</v>
-      </c>
       <c r="Z31" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA31" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB31" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC31" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="6">
@@ -1623,12 +1610,12 @@
       <c r="AA32" s="11"/>
       <c r="AB32" s="11"/>
       <c r="AC32" s="11"/>
-      <c r="AD32" s="19" t="s">
+      <c r="AD32" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="6">
         <v>2</v>
       </c>
@@ -1663,10 +1650,10 @@
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
       <c r="AC33" s="11"/>
-      <c r="AD33" s="19"/>
+      <c r="AD33" s="21"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="6">
         <v>3</v>
       </c>
@@ -1701,10 +1688,10 @@
       <c r="AA34" s="11"/>
       <c r="AB34" s="11"/>
       <c r="AC34" s="11"/>
-      <c r="AD34" s="19"/>
+      <c r="AD34" s="21"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="5">
@@ -1771,12 +1758,12 @@
       <c r="AA35" s="12"/>
       <c r="AB35" s="12"/>
       <c r="AC35" s="12"/>
-      <c r="AD35" s="19" t="s">
+      <c r="AD35" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="5">
         <v>5</v>
       </c>
@@ -1811,10 +1798,10 @@
       <c r="AA36" s="12"/>
       <c r="AB36" s="12"/>
       <c r="AC36" s="12"/>
-      <c r="AD36" s="19"/>
+      <c r="AD36" s="21"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="5">
         <v>6</v>
       </c>
@@ -1849,10 +1836,10 @@
       <c r="AA37" s="12"/>
       <c r="AB37" s="12"/>
       <c r="AC37" s="12"/>
-      <c r="AD37" s="19"/>
+      <c r="AD37" s="21"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="2">
@@ -1889,12 +1876,12 @@
       </c>
       <c r="AB38" s="13"/>
       <c r="AC38" s="13"/>
-      <c r="AD38" s="19" t="s">
+      <c r="AD38" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="2">
         <v>8</v>
       </c>
@@ -1929,10 +1916,10 @@
         <v>1</v>
       </c>
       <c r="AC39" s="14"/>
-      <c r="AD39" s="19"/>
+      <c r="AD39" s="21"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="2">
         <v>9</v>
       </c>
@@ -1967,13 +1954,13 @@
       <c r="AC40" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="AD40" s="19"/>
+      <c r="AD40" s="21"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="L43" s="1">
         <v>1</v>
       </c>
-      <c r="V43" s="8">
+      <c r="Z43" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1987,7 +1974,7 @@
       <c r="E44" s="8">
         <v>3</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="1">
         <v>4</v>
       </c>
       <c r="G44" s="1">
@@ -2027,41 +2014,41 @@
         <v>6</v>
       </c>
       <c r="S44" s="1">
+        <v>3</v>
+      </c>
+      <c r="T44" s="1">
+        <v>4</v>
+      </c>
+      <c r="U44" s="8">
+        <v>5</v>
+      </c>
+      <c r="V44" s="8">
+        <v>6</v>
+      </c>
+      <c r="W44" s="8">
         <v>7</v>
       </c>
-      <c r="T44" s="1">
+      <c r="X44" s="1">
         <v>8</v>
       </c>
-      <c r="U44" s="8">
+      <c r="Y44" s="1">
         <v>9</v>
       </c>
-      <c r="V44" s="8">
-        <v>0</v>
-      </c>
-      <c r="W44" s="8">
-        <v>1</v>
-      </c>
-      <c r="X44" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y44" s="1">
-        <v>3</v>
-      </c>
       <c r="Z44" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA44" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB44" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC44" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="6">
@@ -2100,12 +2087,12 @@
       </c>
       <c r="AB45" s="11"/>
       <c r="AC45" s="11"/>
-      <c r="AD45" s="19" t="s">
+      <c r="AD45" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="6">
         <v>2</v>
       </c>
@@ -2142,10 +2129,10 @@
       </c>
       <c r="AB46" s="11"/>
       <c r="AC46" s="11"/>
-      <c r="AD46" s="19"/>
+      <c r="AD46" s="21"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="6">
         <v>3</v>
       </c>
@@ -2182,10 +2169,10 @@
       </c>
       <c r="AB47" s="11"/>
       <c r="AC47" s="11"/>
-      <c r="AD47" s="19"/>
+      <c r="AD47" s="21"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B48" s="5">
@@ -2254,12 +2241,12 @@
       </c>
       <c r="AB48" s="12"/>
       <c r="AC48" s="12"/>
-      <c r="AD48" s="19" t="s">
+      <c r="AD48" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="5">
         <v>5</v>
       </c>
@@ -2296,10 +2283,10 @@
       </c>
       <c r="AB49" s="12"/>
       <c r="AC49" s="12"/>
-      <c r="AD49" s="19"/>
+      <c r="AD49" s="21"/>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="5">
         <v>6</v>
       </c>
@@ -2336,10 +2323,10 @@
       </c>
       <c r="AB50" s="12"/>
       <c r="AC50" s="12"/>
-      <c r="AD50" s="19"/>
+      <c r="AD50" s="21"/>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="2">
@@ -2380,12 +2367,12 @@
       <c r="AC51" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AD51" s="19" t="s">
+      <c r="AD51" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="2">
         <v>8</v>
       </c>
@@ -2418,10 +2405,10 @@
       <c r="AA52" s="13"/>
       <c r="AB52" s="13"/>
       <c r="AC52" s="14"/>
-      <c r="AD52" s="19"/>
+      <c r="AD52" s="21"/>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="2">
         <v>9</v>
       </c>
@@ -2454,13 +2441,13 @@
       <c r="AA53" s="13"/>
       <c r="AB53" s="14"/>
       <c r="AC53" s="13"/>
-      <c r="AD53" s="19"/>
+      <c r="AD53" s="21"/>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="L57" s="1">
         <v>1</v>
       </c>
-      <c r="V57" s="8">
+      <c r="Z57" s="8">
         <v>2</v>
       </c>
     </row>
@@ -2474,7 +2461,7 @@
       <c r="E58" s="8">
         <v>3</v>
       </c>
-      <c r="F58" s="8">
+      <c r="F58" s="1">
         <v>4</v>
       </c>
       <c r="G58" s="1">
@@ -2514,41 +2501,41 @@
         <v>6</v>
       </c>
       <c r="S58" s="1">
+        <v>3</v>
+      </c>
+      <c r="T58" s="1">
+        <v>4</v>
+      </c>
+      <c r="U58" s="8">
+        <v>5</v>
+      </c>
+      <c r="V58" s="8">
+        <v>6</v>
+      </c>
+      <c r="W58" s="8">
         <v>7</v>
       </c>
-      <c r="T58" s="1">
+      <c r="X58" s="1">
         <v>8</v>
       </c>
-      <c r="U58" s="8">
+      <c r="Y58" s="1">
         <v>9</v>
       </c>
-      <c r="V58" s="8">
-        <v>0</v>
-      </c>
-      <c r="W58" s="8">
-        <v>1</v>
-      </c>
-      <c r="X58" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y58" s="1">
-        <v>3</v>
-      </c>
       <c r="Z58" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA58" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB58" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC58" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="6">
@@ -2589,12 +2576,12 @@
       </c>
       <c r="AB59" s="11"/>
       <c r="AC59" s="11"/>
-      <c r="AD59" s="19" t="s">
+      <c r="AD59" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="6">
         <v>2</v>
       </c>
@@ -2633,10 +2620,10 @@
       </c>
       <c r="AB60" s="11"/>
       <c r="AC60" s="11"/>
-      <c r="AD60" s="19"/>
+      <c r="AD60" s="21"/>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="6">
         <v>3</v>
       </c>
@@ -2675,10 +2662,10 @@
       </c>
       <c r="AB61" s="11"/>
       <c r="AC61" s="11"/>
-      <c r="AD61" s="19"/>
+      <c r="AD61" s="21"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B62" s="5">
@@ -2753,12 +2740,12 @@
       </c>
       <c r="AB62" s="12"/>
       <c r="AC62" s="12"/>
-      <c r="AD62" s="19" t="s">
+      <c r="AD62" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="5">
         <v>5</v>
       </c>
@@ -2795,10 +2782,10 @@
       </c>
       <c r="AB63" s="12"/>
       <c r="AC63" s="12"/>
-      <c r="AD63" s="19"/>
+      <c r="AD63" s="21"/>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A64" s="19"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="5">
         <v>6</v>
       </c>
@@ -2835,10 +2822,10 @@
       </c>
       <c r="AB64" s="12"/>
       <c r="AC64" s="12"/>
-      <c r="AD64" s="19"/>
+      <c r="AD64" s="21"/>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B65" s="2">
@@ -2883,12 +2870,12 @@
       <c r="AC65" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AD65" s="19" t="s">
+      <c r="AD65" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A66" s="19"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="2">
         <v>8</v>
       </c>
@@ -2921,10 +2908,10 @@
       <c r="AA66" s="13"/>
       <c r="AB66" s="13"/>
       <c r="AC66" s="14"/>
-      <c r="AD66" s="19"/>
+      <c r="AD66" s="21"/>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="2">
         <v>9</v>
       </c>
@@ -2957,13 +2944,13 @@
       <c r="AA67" s="13"/>
       <c r="AB67" s="14"/>
       <c r="AC67" s="13"/>
-      <c r="AD67" s="19"/>
+      <c r="AD67" s="21"/>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="L78" s="1">
         <v>1</v>
       </c>
-      <c r="V78" s="8">
+      <c r="Z78" s="8">
         <v>2</v>
       </c>
     </row>
@@ -3017,41 +3004,41 @@
         <v>6</v>
       </c>
       <c r="S79" s="1">
+        <v>3</v>
+      </c>
+      <c r="T79" s="1">
+        <v>4</v>
+      </c>
+      <c r="U79" s="8">
+        <v>5</v>
+      </c>
+      <c r="V79" s="8">
+        <v>6</v>
+      </c>
+      <c r="W79" s="8">
         <v>7</v>
       </c>
-      <c r="T79" s="1">
+      <c r="X79" s="1">
         <v>8</v>
       </c>
-      <c r="U79" s="8">
+      <c r="Y79" s="1">
         <v>9</v>
       </c>
-      <c r="V79" s="8">
-        <v>0</v>
-      </c>
-      <c r="W79" s="8">
-        <v>1</v>
-      </c>
-      <c r="X79" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y79" s="1">
-        <v>3</v>
-      </c>
       <c r="Z79" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA79" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB79" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC79" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B80" s="7">
@@ -3088,13 +3075,13 @@
       </c>
       <c r="AB80" s="11"/>
       <c r="AC80" s="11"/>
-      <c r="AD80" s="19" t="s">
+      <c r="AD80" s="21" t="s">
         <v>7</v>
       </c>
       <c r="AE80" s="7"/>
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A81" s="19"/>
+      <c r="A81" s="21"/>
       <c r="B81" s="7">
         <v>2</v>
       </c>
@@ -3129,11 +3116,11 @@
       </c>
       <c r="AB81" s="11"/>
       <c r="AC81" s="11"/>
-      <c r="AD81" s="19"/>
+      <c r="AD81" s="21"/>
       <c r="AE81" s="7"/>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A82" s="19"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="7">
         <v>3</v>
       </c>
@@ -3168,11 +3155,11 @@
       </c>
       <c r="AB82" s="11"/>
       <c r="AC82" s="11"/>
-      <c r="AD82" s="19"/>
+      <c r="AD82" s="21"/>
       <c r="AE82" s="7"/>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B83" s="5">
@@ -3209,12 +3196,12 @@
       </c>
       <c r="AB83" s="12"/>
       <c r="AC83" s="12"/>
-      <c r="AD83" s="19" t="s">
+      <c r="AD83" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="5">
         <v>5</v>
       </c>
@@ -3249,10 +3236,10 @@
       </c>
       <c r="AB84" s="12"/>
       <c r="AC84" s="12"/>
-      <c r="AD84" s="19"/>
+      <c r="AD84" s="21"/>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
+      <c r="A85" s="21"/>
       <c r="B85" s="5">
         <v>6</v>
       </c>
@@ -3287,10 +3274,10 @@
       </c>
       <c r="AB85" s="12"/>
       <c r="AC85" s="12"/>
-      <c r="AD85" s="19"/>
+      <c r="AD85" s="21"/>
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B86" s="2">
@@ -3369,12 +3356,12 @@
       </c>
       <c r="AB86" s="13"/>
       <c r="AC86" s="13"/>
-      <c r="AD86" s="19" t="s">
+      <c r="AD86" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A87" s="19"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="2">
         <v>8</v>
       </c>
@@ -3409,10 +3396,10 @@
         <v>1</v>
       </c>
       <c r="AC87" s="14"/>
-      <c r="AD87" s="19"/>
+      <c r="AD87" s="21"/>
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A88" s="19"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="2">
         <v>9</v>
       </c>
@@ -3447,13 +3434,13 @@
       <c r="AC88" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="AD88" s="19"/>
+      <c r="AD88" s="21"/>
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.25">
       <c r="L94" s="1">
         <v>1</v>
       </c>
-      <c r="V94" s="8">
+      <c r="Z94" s="8">
         <v>2</v>
       </c>
     </row>
@@ -3507,41 +3494,41 @@
         <v>6</v>
       </c>
       <c r="S95" s="1">
+        <v>3</v>
+      </c>
+      <c r="T95" s="1">
+        <v>4</v>
+      </c>
+      <c r="U95" s="8">
+        <v>5</v>
+      </c>
+      <c r="V95" s="8">
+        <v>6</v>
+      </c>
+      <c r="W95" s="8">
         <v>7</v>
       </c>
-      <c r="T95" s="1">
+      <c r="X95" s="1">
         <v>8</v>
       </c>
-      <c r="U95" s="8">
+      <c r="Y95" s="1">
         <v>9</v>
       </c>
-      <c r="V95" s="8">
-        <v>0</v>
-      </c>
-      <c r="W95" s="8">
-        <v>1</v>
-      </c>
-      <c r="X95" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y95" s="1">
-        <v>3</v>
-      </c>
       <c r="Z95" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA95" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB95" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC95" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A96" s="19" t="s">
+      <c r="A96" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B96" s="6">
@@ -3578,12 +3565,12 @@
       <c r="AA96" s="11"/>
       <c r="AB96" s="11"/>
       <c r="AC96" s="11"/>
-      <c r="AD96" s="19" t="s">
+      <c r="AD96" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A97" s="19"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="6">
         <v>2</v>
       </c>
@@ -3618,10 +3605,10 @@
       <c r="AA97" s="11"/>
       <c r="AB97" s="11"/>
       <c r="AC97" s="11"/>
-      <c r="AD97" s="19"/>
+      <c r="AD97" s="21"/>
     </row>
     <row r="98" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A98" s="19"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="6">
         <v>3</v>
       </c>
@@ -3656,10 +3643,10 @@
       <c r="AA98" s="11"/>
       <c r="AB98" s="11"/>
       <c r="AC98" s="11"/>
-      <c r="AD98" s="19"/>
+      <c r="AD98" s="21"/>
     </row>
     <row r="99" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A99" s="19" t="s">
+      <c r="A99" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B99" s="5">
@@ -3696,12 +3683,12 @@
       <c r="AA99" s="12"/>
       <c r="AB99" s="12"/>
       <c r="AC99" s="12"/>
-      <c r="AD99" s="19" t="s">
+      <c r="AD99" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A100" s="19"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="5">
         <v>5</v>
       </c>
@@ -3736,10 +3723,10 @@
       <c r="AA100" s="12"/>
       <c r="AB100" s="12"/>
       <c r="AC100" s="12"/>
-      <c r="AD100" s="19"/>
+      <c r="AD100" s="21"/>
     </row>
     <row r="101" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A101" s="19"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="5">
         <v>6</v>
       </c>
@@ -3774,10 +3761,10 @@
       <c r="AA101" s="12"/>
       <c r="AB101" s="12"/>
       <c r="AC101" s="12"/>
-      <c r="AD101" s="19"/>
+      <c r="AD101" s="21"/>
     </row>
     <row r="102" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A102" s="19" t="s">
+      <c r="A102" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B102" s="2">
@@ -3862,12 +3849,12 @@
       <c r="AC102" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AD102" s="19" t="s">
+      <c r="AD102" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A103" s="19"/>
+      <c r="A103" s="21"/>
       <c r="B103" s="2">
         <v>8</v>
       </c>
@@ -3898,10 +3885,10 @@
       <c r="AA103" s="13"/>
       <c r="AB103" s="13"/>
       <c r="AC103" s="14"/>
-      <c r="AD103" s="19"/>
+      <c r="AD103" s="21"/>
     </row>
     <row r="104" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A104" s="19"/>
+      <c r="A104" s="21"/>
       <c r="B104" s="2">
         <v>9</v>
       </c>
@@ -3932,7 +3919,7 @@
       <c r="AA104" s="13"/>
       <c r="AB104" s="14"/>
       <c r="AC104" s="13"/>
-      <c r="AD104" s="19"/>
+      <c r="AD104" s="21"/>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G106" s="4" t="s">
@@ -3945,6 +3932,14 @@
     <row r="108" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G108" s="3"/>
     </row>
+    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L109" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z109" s="8">
+        <v>2</v>
+      </c>
+    </row>
     <row r="110" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C110" s="9">
         <v>1</v>
@@ -3995,41 +3990,41 @@
         <v>6</v>
       </c>
       <c r="S110" s="1">
+        <v>3</v>
+      </c>
+      <c r="T110" s="1">
+        <v>4</v>
+      </c>
+      <c r="U110" s="8">
+        <v>5</v>
+      </c>
+      <c r="V110" s="8">
+        <v>6</v>
+      </c>
+      <c r="W110" s="8">
         <v>7</v>
       </c>
-      <c r="T110" s="1">
+      <c r="X110" s="1">
         <v>8</v>
       </c>
-      <c r="U110" s="8">
+      <c r="Y110" s="1">
         <v>9</v>
       </c>
-      <c r="V110" s="8">
-        <v>0</v>
-      </c>
-      <c r="W110" s="8">
-        <v>1</v>
-      </c>
-      <c r="X110" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y110" s="1">
-        <v>3</v>
-      </c>
       <c r="Z110" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA110" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB110" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC110" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A111" s="19" t="s">
+      <c r="A111" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B111" s="6">
@@ -4066,12 +4061,12 @@
       <c r="AA111" s="11"/>
       <c r="AB111" s="11"/>
       <c r="AC111" s="11"/>
-      <c r="AD111" s="19" t="s">
+      <c r="AD111" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A112" s="19"/>
+      <c r="A112" s="21"/>
       <c r="B112" s="6">
         <v>2</v>
       </c>
@@ -4106,13 +4101,13 @@
       <c r="AA112" s="11"/>
       <c r="AB112" s="11"/>
       <c r="AC112" s="11"/>
-      <c r="AD112" s="19"/>
+      <c r="AD112" s="21"/>
       <c r="AF112" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A113" s="19"/>
+      <c r="A113" s="21"/>
       <c r="B113" s="6">
         <v>3</v>
       </c>
@@ -4147,10 +4142,10 @@
       <c r="AA113" s="11"/>
       <c r="AB113" s="11"/>
       <c r="AC113" s="11"/>
-      <c r="AD113" s="19"/>
+      <c r="AD113" s="21"/>
     </row>
     <row r="114" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A114" s="19" t="s">
+      <c r="A114" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B114" s="5">
@@ -4187,12 +4182,12 @@
       <c r="AA114" s="12"/>
       <c r="AB114" s="12"/>
       <c r="AC114" s="12"/>
-      <c r="AD114" s="19" t="s">
+      <c r="AD114" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A115" s="19"/>
+      <c r="A115" s="21"/>
       <c r="B115" s="5">
         <v>5</v>
       </c>
@@ -4227,13 +4222,13 @@
       <c r="AA115" s="12"/>
       <c r="AB115" s="12"/>
       <c r="AC115" s="12"/>
-      <c r="AD115" s="19"/>
+      <c r="AD115" s="21"/>
       <c r="AF115" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A116" s="19"/>
+      <c r="A116" s="21"/>
       <c r="B116" s="5">
         <v>6</v>
       </c>
@@ -4268,10 +4263,10 @@
       <c r="AA116" s="12"/>
       <c r="AB116" s="12"/>
       <c r="AC116" s="12"/>
-      <c r="AD116" s="19"/>
+      <c r="AD116" s="21"/>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A117" s="19" t="s">
+      <c r="A117" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B117" s="2">
@@ -4308,12 +4303,12 @@
       </c>
       <c r="AB117" s="13"/>
       <c r="AC117" s="13"/>
-      <c r="AD117" s="19" t="s">
+      <c r="AD117" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A118" s="19"/>
+      <c r="A118" s="21"/>
       <c r="B118" s="2">
         <v>8</v>
       </c>
@@ -4348,13 +4343,13 @@
         <v>1</v>
       </c>
       <c r="AC118" s="14"/>
-      <c r="AD118" s="19"/>
+      <c r="AD118" s="21"/>
       <c r="AF118" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A119" s="19"/>
+      <c r="A119" s="21"/>
       <c r="B119" s="2">
         <v>9</v>
       </c>
@@ -4389,58 +4384,533 @@
       <c r="AC119" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="AD119" s="19"/>
+      <c r="AD119" s="21"/>
+    </row>
+    <row r="124" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L124" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z124" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C125" s="9">
+        <v>1</v>
+      </c>
+      <c r="D125" s="8">
+        <v>2</v>
+      </c>
+      <c r="E125" s="8">
+        <v>3</v>
+      </c>
+      <c r="F125" s="1">
+        <v>4</v>
+      </c>
+      <c r="G125" s="1">
+        <v>5</v>
+      </c>
+      <c r="H125" s="1">
+        <v>6</v>
+      </c>
+      <c r="I125" s="8">
+        <v>7</v>
+      </c>
+      <c r="J125" s="8">
+        <v>8</v>
+      </c>
+      <c r="K125" s="8">
+        <v>9</v>
+      </c>
+      <c r="L125" s="1">
+        <v>0</v>
+      </c>
+      <c r="M125" s="1">
+        <v>1</v>
+      </c>
+      <c r="N125" s="1">
+        <v>2</v>
+      </c>
+      <c r="O125" s="8">
+        <v>3</v>
+      </c>
+      <c r="P125" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q125" s="8">
+        <v>5</v>
+      </c>
+      <c r="R125" s="1">
+        <v>6</v>
+      </c>
+      <c r="S125" s="1">
+        <v>3</v>
+      </c>
+      <c r="T125" s="1">
+        <v>4</v>
+      </c>
+      <c r="U125" s="8">
+        <v>5</v>
+      </c>
+      <c r="V125" s="8">
+        <v>6</v>
+      </c>
+      <c r="W125" s="8">
+        <v>7</v>
+      </c>
+      <c r="X125" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y125" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z125" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA125" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB125" s="8">
+        <v>2</v>
+      </c>
+      <c r="AC125" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A126" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="6">
+        <v>1</v>
+      </c>
+      <c r="C126" s="10"/>
+      <c r="D126" s="11"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I126" s="13"/>
+      <c r="J126" s="13"/>
+      <c r="K126" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L126" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M126" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N126" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O126" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="P126" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q126" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="R126" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="S126" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="T126" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="U126" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="V126" s="13"/>
+      <c r="W126" s="13"/>
+      <c r="X126" s="12"/>
+      <c r="Y126" s="12"/>
+      <c r="Z126" s="12"/>
+      <c r="AA126" s="11"/>
+      <c r="AB126" s="11"/>
+      <c r="AC126" s="11"/>
+      <c r="AD126" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A127" s="21"/>
+      <c r="B127" s="6">
+        <v>2</v>
+      </c>
+      <c r="C127" s="10"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="12"/>
+      <c r="H127" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I127" s="13"/>
+      <c r="J127" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K127" s="13"/>
+      <c r="L127" s="16"/>
+      <c r="M127" s="16"/>
+      <c r="N127" s="16"/>
+      <c r="O127" s="17"/>
+      <c r="P127" s="17"/>
+      <c r="Q127" s="17"/>
+      <c r="R127" s="16"/>
+      <c r="S127" s="16"/>
+      <c r="T127" s="16"/>
+      <c r="U127" s="13"/>
+      <c r="V127" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="W127" s="13"/>
+      <c r="X127" s="12"/>
+      <c r="Y127" s="12"/>
+      <c r="Z127" s="12"/>
+      <c r="AA127" s="11"/>
+      <c r="AB127" s="11"/>
+      <c r="AC127" s="11"/>
+      <c r="AD127" s="21"/>
+    </row>
+    <row r="128" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A128" s="21"/>
+      <c r="B128" s="6">
+        <v>3</v>
+      </c>
+      <c r="C128" s="10"/>
+      <c r="D128" s="11"/>
+      <c r="E128" s="11"/>
+      <c r="F128" s="12"/>
+      <c r="G128" s="12"/>
+      <c r="H128" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I128" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J128" s="13"/>
+      <c r="K128" s="13"/>
+      <c r="L128" s="16"/>
+      <c r="M128" s="16"/>
+      <c r="N128" s="16"/>
+      <c r="O128" s="17"/>
+      <c r="P128" s="17"/>
+      <c r="Q128" s="17"/>
+      <c r="R128" s="16"/>
+      <c r="S128" s="16"/>
+      <c r="T128" s="16"/>
+      <c r="U128" s="13"/>
+      <c r="V128" s="13"/>
+      <c r="W128" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="X128" s="12"/>
+      <c r="Y128" s="12"/>
+      <c r="Z128" s="12"/>
+      <c r="AA128" s="11"/>
+      <c r="AB128" s="11"/>
+      <c r="AC128" s="11"/>
+      <c r="AD128" s="21"/>
+    </row>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A129" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B129" s="5">
+        <v>4</v>
+      </c>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I129" s="16"/>
+      <c r="J129" s="16"/>
+      <c r="K129" s="16"/>
+      <c r="L129" s="17"/>
+      <c r="M129" s="17"/>
+      <c r="N129" s="17"/>
+      <c r="O129" s="11"/>
+      <c r="P129" s="11"/>
+      <c r="Q129" s="11"/>
+      <c r="R129" s="17"/>
+      <c r="S129" s="17"/>
+      <c r="T129" s="17"/>
+      <c r="U129" s="15"/>
+      <c r="V129" s="16"/>
+      <c r="W129" s="16"/>
+      <c r="X129" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y129" s="13"/>
+      <c r="Z129" s="13"/>
+      <c r="AA129" s="12"/>
+      <c r="AB129" s="12"/>
+      <c r="AC129" s="12"/>
+      <c r="AD129" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A130" s="21"/>
+      <c r="B130" s="5">
+        <v>5</v>
+      </c>
+      <c r="C130" s="12"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="13"/>
+      <c r="G130" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H130" s="13"/>
+      <c r="I130" s="16"/>
+      <c r="J130" s="16"/>
+      <c r="K130" s="16"/>
+      <c r="L130" s="17"/>
+      <c r="M130" s="17"/>
+      <c r="N130" s="17"/>
+      <c r="O130" s="11"/>
+      <c r="P130" s="11"/>
+      <c r="Q130" s="11"/>
+      <c r="R130" s="17"/>
+      <c r="S130" s="17"/>
+      <c r="T130" s="17"/>
+      <c r="U130" s="16"/>
+      <c r="V130" s="16"/>
+      <c r="W130" s="16"/>
+      <c r="X130" s="13"/>
+      <c r="Y130" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z130" s="14"/>
+      <c r="AA130" s="12"/>
+      <c r="AB130" s="12"/>
+      <c r="AC130" s="12"/>
+      <c r="AD130" s="21"/>
+    </row>
+    <row r="131" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A131" s="21"/>
+      <c r="B131" s="5">
+        <v>6</v>
+      </c>
+      <c r="C131" s="12"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="16"/>
+      <c r="J131" s="16"/>
+      <c r="K131" s="16"/>
+      <c r="L131" s="17"/>
+      <c r="M131" s="17"/>
+      <c r="N131" s="17"/>
+      <c r="O131" s="11"/>
+      <c r="P131" s="11"/>
+      <c r="Q131" s="11"/>
+      <c r="R131" s="17"/>
+      <c r="S131" s="17"/>
+      <c r="T131" s="17"/>
+      <c r="U131" s="16"/>
+      <c r="V131" s="16"/>
+      <c r="W131" s="16"/>
+      <c r="X131" s="13"/>
+      <c r="Y131" s="14"/>
+      <c r="Z131" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA131" s="12"/>
+      <c r="AB131" s="12"/>
+      <c r="AC131" s="12"/>
+      <c r="AD131" s="21"/>
+    </row>
+    <row r="132" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A132" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B132" s="2">
+        <v>7</v>
+      </c>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16"/>
+      <c r="H132" s="16"/>
+      <c r="I132" s="17"/>
+      <c r="J132" s="17"/>
+      <c r="K132" s="17"/>
+      <c r="L132" s="11"/>
+      <c r="M132" s="11"/>
+      <c r="N132" s="11"/>
+      <c r="O132" s="12"/>
+      <c r="P132" s="12"/>
+      <c r="Q132" s="12"/>
+      <c r="R132" s="11"/>
+      <c r="S132" s="11"/>
+      <c r="T132" s="11"/>
+      <c r="U132" s="17"/>
+      <c r="V132" s="17"/>
+      <c r="W132" s="17"/>
+      <c r="X132" s="15"/>
+      <c r="Y132" s="16"/>
+      <c r="Z132" s="16"/>
+      <c r="AA132" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB132" s="13"/>
+      <c r="AC132" s="13"/>
+      <c r="AD132" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A133" s="21"/>
+      <c r="B133" s="2">
+        <v>8</v>
+      </c>
+      <c r="C133" s="13"/>
+      <c r="D133" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E133" s="13"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="16"/>
+      <c r="I133" s="17"/>
+      <c r="J133" s="17"/>
+      <c r="K133" s="17"/>
+      <c r="L133" s="11"/>
+      <c r="M133" s="11"/>
+      <c r="N133" s="11"/>
+      <c r="O133" s="12"/>
+      <c r="P133" s="12"/>
+      <c r="Q133" s="12"/>
+      <c r="R133" s="11"/>
+      <c r="S133" s="11"/>
+      <c r="T133" s="11"/>
+      <c r="U133" s="17"/>
+      <c r="V133" s="17"/>
+      <c r="W133" s="17"/>
+      <c r="X133" s="16"/>
+      <c r="Y133" s="16"/>
+      <c r="Z133" s="16"/>
+      <c r="AA133" s="13"/>
+      <c r="AB133" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC133" s="14"/>
+      <c r="AD133" s="21"/>
+    </row>
+    <row r="134" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A134" s="21"/>
+      <c r="B134" s="2">
+        <v>9</v>
+      </c>
+      <c r="C134" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="16"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="16"/>
+      <c r="I134" s="17"/>
+      <c r="J134" s="17"/>
+      <c r="K134" s="17"/>
+      <c r="L134" s="11"/>
+      <c r="M134" s="11"/>
+      <c r="N134" s="11"/>
+      <c r="O134" s="12"/>
+      <c r="P134" s="12"/>
+      <c r="Q134" s="12"/>
+      <c r="R134" s="11"/>
+      <c r="S134" s="11"/>
+      <c r="T134" s="11"/>
+      <c r="U134" s="17"/>
+      <c r="V134" s="17"/>
+      <c r="W134" s="17"/>
+      <c r="X134" s="16"/>
+      <c r="Y134" s="16"/>
+      <c r="Z134" s="16"/>
+      <c r="AA134" s="13"/>
+      <c r="AB134" s="14"/>
+      <c r="AC134" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD134" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="54">
+    <mergeCell ref="A126:A128"/>
+    <mergeCell ref="AD126:AD128"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="AD129:AD131"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="AD132:AD134"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="AD111:AD113"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="AD114:AD116"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="AD117:AD119"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="AD19:AD21"/>
+    <mergeCell ref="AD22:AD24"/>
+    <mergeCell ref="AD25:AD27"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="AD32:AD34"/>
+    <mergeCell ref="AD35:AD37"/>
+    <mergeCell ref="AD38:AD40"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="AD45:AD47"/>
+    <mergeCell ref="AD48:AD50"/>
+    <mergeCell ref="AD51:AD53"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="AD59:AD61"/>
+    <mergeCell ref="AD62:AD64"/>
+    <mergeCell ref="AD65:AD67"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="AD80:AD82"/>
+    <mergeCell ref="AD83:AD85"/>
+    <mergeCell ref="AD86:AD88"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="AD96:AD98"/>
+    <mergeCell ref="AD99:AD101"/>
+    <mergeCell ref="AD102:AD104"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="AD3:AD5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="AD6:AD8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="AD9:AD11"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="AD96:AD98"/>
-    <mergeCell ref="AD99:AD101"/>
-    <mergeCell ref="AD102:AD104"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="AD80:AD82"/>
-    <mergeCell ref="AD83:AD85"/>
-    <mergeCell ref="AD86:AD88"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="AD59:AD61"/>
-    <mergeCell ref="AD62:AD64"/>
-    <mergeCell ref="AD65:AD67"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="AD45:AD47"/>
-    <mergeCell ref="AD48:AD50"/>
-    <mergeCell ref="AD51:AD53"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="AD32:AD34"/>
-    <mergeCell ref="AD35:AD37"/>
-    <mergeCell ref="AD38:AD40"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="AD19:AD21"/>
-    <mergeCell ref="AD22:AD24"/>
-    <mergeCell ref="AD25:AD27"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="AD111:AD113"/>
-    <mergeCell ref="A114:A116"/>
-    <mergeCell ref="AD114:AD116"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="AD117:AD119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>